<commit_message>
Truly the end, probably
</commit_message>
<xml_diff>
--- a/333 Project/Spreadsheets/5eClasses.xlsx
+++ b/333 Project/Spreadsheets/5eClasses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansarij\Documents\333 Classwork\Project\Git\333 Project\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC94542E-1864-40A2-A34A-05AFA06014DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4DA0E5-0B3A-417D-BB65-060D1E38D8DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="732" yWindow="732" windowWidth="17292" windowHeight="9420" xr2:uid="{9E08A55B-82BB-4D5F-A0E6-14761A231183}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Class Description</t>
   </si>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>Rogue</t>
-  </si>
-  <si>
-    <t>Blood Hunter</t>
   </si>
   <si>
     <t>Barbarians are defined by their rage: unbridled, unquenchable, and unthinking fury. More than a mere emotion, their anger is the ferocity of a cornered predator, the unrelenting assault of a storm, the churning turmoil of the sea.
@@ -86,9 +83,6 @@
   </si>
   <si>
     <t>In the worlds of D&amp;D, words and music are not just vibrations of air, but vocalizations with power all their own. The bard is a master of song, speech, and the magic they contain. Bards say that the multiverse was spoken into existence, that the words of the gods gave it shape, and that echoes of these primordial Words of Creation still resound throughout the cosmos. The music of bards is an attempt to snatch and harness those echoes, subtly woven into their spells and powers. The greatest strength of bards is their sheer versatility. Many bards prefer to stick to the sidelines in combat, using their magic to inspire their allies and hinder their foes from a distance. But bards are capable of defending themselves in melee if necessary, using their magic to bolster their swords and armor. Their spells lean toward charms and illusions rather than blatantly destructive spells. They have a wide-ranging knowledge of many subjects and a natural aptitude that lets them do almost anything well. Bards become masters of the talents they set their minds to perfecting, from musical performance to esoteric knowledge.</t>
-  </si>
-  <si>
-    <t>Often feared or misunderstood, and driven by an unending drive to destroy the wicked, blood hunters are clever, arcane warriors who have bound their essence to the dark creatures they hunt to better stalk and survive their prey. Armed with the rites of forbidden blood magic and a willingness to sacrifice their own vitality and humanity for the cause, they protect the realms from the shadows, ever vigilant to avoid becoming the same monsters they choose to hunt.</t>
   </si>
   <si>
     <t>Clerics are intermediaries between the mortal world and the distant planes of the gods. As varied as the gods they serve, clerics strive to embody the handiwork of their deities. No ordinary priest, a cleric is imbued with divine magic. Divine magic, as the name suggests, is the power of the gods, flowing from them into the world. Clerics are conduits for that power, manifesting it as miraculous effects. The gods don’t grant this power to everyone who seeks it, but only to those chosen to fulfill a high calling. Harnessing divine magic doesn’t rely on study or training. A cleric might learn formulaic prayers and ancient rites, but the ability to cast cleric spells relies on devotion and an intuitive sense of a deity’s wishes. Clerics combine the helpful magic of healing and inspiring their allies with spells that harm and hinder foes. They can provoke awe and dread, lay curses of plague or poison, and even call down flames from heaven to consume their enemies. For those evildoers who will benefit most from a mace to the head, clerics depend on their combat training to let them wade into melee with the power of the gods on their side.</t>
@@ -486,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A04A728-3F02-4B65-A4CE-C7A504CED0D5}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B14"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,7 +505,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -519,95 +513,87 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>